<commit_message>
Upload test report of success story list page. (Kaii)
</commit_message>
<xml_diff>
--- a/PCB/04 Dev_Lib/4.4_Unit Test/Unit Test (Success Story List)_v0.1.xlsx
+++ b/PCB/04 Dev_Lib/4.4_Unit Test/Unit Test (Success Story List)_v0.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="345" windowWidth="19875" windowHeight="7725"/>
+    <workbookView xWindow="45" yWindow="-30" windowWidth="12345" windowHeight="7725"/>
   </bookViews>
   <sheets>
     <sheet name="Test(List)" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="51">
   <si>
     <t>Page</t>
   </si>
@@ -37,9 +37,6 @@
     <t>Test Result</t>
   </si>
   <si>
-    <t>Y/N</t>
-  </si>
-  <si>
     <t>Test Date</t>
   </si>
   <si>
@@ -91,10 +88,6 @@
     <t>Sort Order</t>
   </si>
   <si>
-    <t xml:space="preserve">Success story list should be sorted in the order of "SortOrder".
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">All the records in list are sorted by "SortOrder" in the DB.
 </t>
   </si>
@@ -188,6 +181,19 @@
   </si>
   <si>
     <t xml:space="preserve">After clicking the link of one success story,  the detail page can be displayed.
+</t>
+  </si>
+  <si>
+    <t>(Y/N)</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Kaii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Success story list should be sorted in the order of "sortOrder".
 </t>
   </si>
 </sst>
@@ -375,20 +381,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -449,6 +443,24 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -751,400 +763,475 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
+      <pane ySplit="4" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="41.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="39.5703125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="29.28515625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="2.7109375" style="6"/>
+    <col min="1" max="1" width="5.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="41.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="39.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="2.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="7"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-    </row>
-    <row r="3" spans="1:9" s="13" customFormat="1">
-      <c r="A3" s="8" t="s">
+      <c r="D1" s="25"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="3"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" s="9" customFormat="1">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="12" t="s">
+    </row>
+    <row r="4" spans="1:8" s="9" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" s="13" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A4" s="14"/>
-      <c r="B4" s="15" t="s">
+      <c r="C4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="D4" s="13"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18" t="s">
+    </row>
+    <row r="5" spans="1:8" ht="27.75" customHeight="1">
+      <c r="A5" s="15">
+        <v>1</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="27.75" customHeight="1">
-      <c r="A5" s="19">
-        <v>1</v>
-      </c>
-      <c r="B5" s="20" t="s">
+      <c r="C5" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="D5" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="E5" s="16"/>
+      <c r="F5" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="27">
+        <v>42277</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="36">
+      <c r="A6" s="15">
+        <v>2</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-    </row>
-    <row r="6" spans="1:9" ht="36">
-      <c r="A6" s="19">
-        <v>2</v>
-      </c>
-      <c r="B6" s="20" t="s">
+      <c r="C6" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="D6" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="E6" s="19"/>
+      <c r="F6" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="27">
+        <v>42277</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="36">
+      <c r="A7" s="15">
+        <v>3</v>
+      </c>
+      <c r="B7" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-    </row>
-    <row r="7" spans="1:9" ht="36">
-      <c r="A7" s="19">
-        <v>3</v>
-      </c>
-      <c r="B7" s="20" t="s">
+      <c r="C7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="D7" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="E7" s="19"/>
+      <c r="F7" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="27">
+        <v>42277</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="36">
+      <c r="A8" s="15">
+        <v>4</v>
+      </c>
+      <c r="B8" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-    </row>
-    <row r="8" spans="1:9" ht="36">
-      <c r="A8" s="19">
-        <v>4</v>
-      </c>
-      <c r="B8" s="24" t="s">
+      <c r="C8" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="E8" s="19"/>
+      <c r="F8" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="27">
+        <v>42279</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="36">
+      <c r="A9" s="15">
+        <v>5</v>
+      </c>
+      <c r="B9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="C9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-    </row>
-    <row r="9" spans="1:9" ht="36">
-      <c r="A9" s="19">
-        <v>5</v>
-      </c>
-      <c r="B9" s="24" t="s">
+      <c r="D9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="E9" s="19"/>
+      <c r="F9" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="27">
+        <v>42277</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="36">
+      <c r="A10" s="15">
+        <v>6</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D10" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-    </row>
-    <row r="10" spans="1:9" ht="36">
-      <c r="A10" s="19">
-        <v>6</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="21" t="s">
+      <c r="E10" s="19"/>
+      <c r="F10" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="27">
+        <v>42277</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="36">
+      <c r="A11" s="15">
+        <v>7</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D11" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-    </row>
-    <row r="11" spans="1:9" ht="36">
-      <c r="A11" s="19">
-        <v>7</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="21" t="s">
+      <c r="E11" s="19"/>
+      <c r="F11" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="27">
+        <v>42277</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="24">
+      <c r="A12" s="15">
+        <v>8</v>
+      </c>
+      <c r="B12" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="C12" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-    </row>
-    <row r="12" spans="1:9" ht="24">
-      <c r="A12" s="19">
-        <v>8</v>
-      </c>
-      <c r="B12" s="24" t="s">
+      <c r="D12" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="E12" s="19"/>
+      <c r="F12" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="27">
+        <v>42277</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="36">
+      <c r="A13" s="15">
+        <v>9</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D13" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-    </row>
-    <row r="13" spans="1:9" ht="36">
-      <c r="A13" s="19">
-        <v>9</v>
-      </c>
-      <c r="B13" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="21" t="s">
+      <c r="E13" s="19"/>
+      <c r="F13" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="27">
+        <v>42277</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="36">
+      <c r="A14" s="15">
+        <v>10</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D14" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-    </row>
-    <row r="14" spans="1:9" ht="36">
-      <c r="A14" s="19">
-        <v>10</v>
-      </c>
-      <c r="B14" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="21" t="s">
+      <c r="E14" s="19"/>
+      <c r="F14" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="27">
+        <v>42277</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="36">
+      <c r="A15" s="15">
+        <v>11</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D15" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-    </row>
-    <row r="15" spans="1:9" ht="36">
-      <c r="A15" s="19">
-        <v>11</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="21" t="s">
+      <c r="E15" s="19"/>
+      <c r="F15" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="27">
+        <v>42279</v>
+      </c>
+      <c r="H15" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="36">
+      <c r="A16" s="15">
+        <v>12</v>
+      </c>
+      <c r="B16" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="C16" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-    </row>
-    <row r="16" spans="1:9" ht="36">
-      <c r="A16" s="19">
-        <v>12</v>
-      </c>
-      <c r="B16" s="24" t="s">
+      <c r="D16" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="E16" s="19"/>
+      <c r="F16" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" s="27">
+        <v>42277</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="36">
+      <c r="A17" s="15">
+        <v>13</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="E17" s="19"/>
+      <c r="F17" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" s="27">
+        <v>42277</v>
+      </c>
+      <c r="H17" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="36">
+      <c r="A18" s="15">
+        <v>14</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-    </row>
-    <row r="17" spans="1:9" ht="36">
-      <c r="A17" s="19">
-        <v>13</v>
-      </c>
-      <c r="B17" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="21" t="s">
+      <c r="E18" s="19"/>
+      <c r="F18" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="27">
+        <v>42277</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="36">
+      <c r="A19" s="15">
+        <v>15</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-    </row>
-    <row r="18" spans="1:9" ht="36">
-      <c r="A18" s="19">
-        <v>14</v>
-      </c>
-      <c r="B18" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="21" t="s">
+      <c r="E19" s="19"/>
+      <c r="F19" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" s="27">
+        <v>42277</v>
+      </c>
+      <c r="H19" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="36">
+      <c r="A20" s="15">
+        <v>16</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-    </row>
-    <row r="19" spans="1:9" ht="36">
-      <c r="A19" s="19">
-        <v>15</v>
-      </c>
-      <c r="B19" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="21" t="s">
+      <c r="D20" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-    </row>
-    <row r="20" spans="1:9" ht="36">
-      <c r="A20" s="19">
-        <v>16</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" s="27">
+        <v>42277</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>